<commit_message>
updating ig with HAICA examples
</commit_message>
<xml_diff>
--- a/StructureDefinition-cbs-case-notification-panel.xlsx
+++ b/StructureDefinition-cbs-case-notification-panel.xlsx
@@ -755,8 +755,8 @@
     <t>Observation.value[x]</t>
   </si>
   <si>
-    <t>CodeableConcept
-stringintegerdateTime</t>
+    <t>Quantity
+CodeableConceptstringintegerdateTime</t>
   </si>
   <si>
     <t>Actual result</t>

</xml_diff>